<commit_message>
better codes implemention needs more accuracy
</commit_message>
<xml_diff>
--- a/src/server/excelFiles/provinces locations code.xlsx
+++ b/src/server/excelFiles/provinces locations code.xlsx
@@ -22,7 +22,7 @@
     <t>province</t>
   </si>
   <si>
-    <t>district</t>
+    <t>district_code</t>
   </si>
   <si>
     <t>english_description</t>
@@ -2958,7 +2958,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -3036,10 +3036,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4962,7 +4962,7 @@
         <v>138</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="19.5">
       <c r="A124" s="5"/>
       <c r="B124" s="5"/>
       <c r="C124" s="6">
@@ -4975,7 +4975,7 @@
         <v>354</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="19.5">
       <c r="A125" s="5"/>
       <c r="B125" s="5"/>
       <c r="C125" s="6">
@@ -4988,7 +4988,7 @@
         <v>356</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="19.5">
       <c r="A126" s="5"/>
       <c r="B126" s="5"/>
       <c r="C126" s="6">
@@ -5001,7 +5001,7 @@
         <v>358</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="19.5">
       <c r="A127" s="5"/>
       <c r="B127" s="5"/>
       <c r="C127" s="6">
@@ -5014,7 +5014,7 @@
         <v>360</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="19.5">
       <c r="A128" s="5"/>
       <c r="B128" s="5"/>
       <c r="C128" s="6">
@@ -5027,7 +5027,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="19.5">
       <c r="A129" s="5"/>
       <c r="B129" s="5"/>
       <c r="C129" s="6">
@@ -5040,7 +5040,7 @@
         <v>362</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="19.5">
       <c r="A130" s="5"/>
       <c r="B130" s="5"/>
       <c r="C130" s="6">
@@ -5053,7 +5053,7 @@
         <v>364</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="19.5">
       <c r="A131" s="5"/>
       <c r="B131" s="5"/>
       <c r="C131" s="6">
@@ -5066,7 +5066,7 @@
         <v>366</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="19.5">
       <c r="A132" s="5"/>
       <c r="B132" s="5"/>
       <c r="C132" s="6">
@@ -5079,7 +5079,7 @@
         <v>368</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="19.5">
       <c r="A133" s="5"/>
       <c r="B133" s="5"/>
       <c r="C133" s="6">
@@ -5092,7 +5092,7 @@
         <v>370</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="19.5">
       <c r="A134" s="5"/>
       <c r="B134" s="5"/>
       <c r="C134" s="6">
@@ -5105,7 +5105,7 @@
         <v>372</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="19.5">
       <c r="A135" s="5"/>
       <c r="B135" s="5"/>
       <c r="C135" s="6">
@@ -5118,7 +5118,7 @@
         <v>374</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="19.5">
       <c r="A136" s="5"/>
       <c r="B136" s="5"/>
       <c r="C136" s="6">
@@ -5131,7 +5131,7 @@
         <v>376</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="19.5">
       <c r="A137" s="5"/>
       <c r="B137" s="5">
         <v>12</v>

</xml_diff>